<commit_message>
Criação de base de dados para o APP
</commit_message>
<xml_diff>
--- a/DashboardModelo1/dadosPlanilha/planilha_saida.xlsx
+++ b/DashboardModelo1/dadosPlanilha/planilha_saida.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sandbox\DashboardCotton\DashboardModelo1\dadosPlanilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B9509C-8DC0-45FB-ABAA-26D3BEEE9C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44737B50-E7C6-4A83-A36A-FBF369B371A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="309">
   <si>
     <t>VARIAVEIS GLOBAIS (GUARDA-CHUVA)</t>
   </si>
@@ -134,15 +134,15 @@
     <t>R$ 1.313,00</t>
   </si>
   <si>
-    <t>1.3 Seguro Maquinario Equipamentos Utilit.</t>
-  </si>
-  <si>
     <t>R$ 1.414,00</t>
   </si>
   <si>
     <t>F. OUTROS CUSTOS (R$)</t>
   </si>
   <si>
+    <t>1.1 Assistência Técnica</t>
+  </si>
+  <si>
     <t>R$ 1.515,00</t>
   </si>
   <si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>R$ 1.919,00</t>
-  </si>
-  <si>
-    <t>1.3 Despesas Gerias</t>
   </si>
   <si>
     <t>R$ 2.020,00</t>
@@ -951,6 +948,12 @@
   </si>
   <si>
     <t>1.2 Temporária</t>
+  </si>
+  <si>
+    <t>1.3 Seguro Maquinário Equipamentos Utilit.</t>
+  </si>
+  <si>
+    <t>1.3 Despesas Gerais</t>
   </si>
 </sst>
 </file>
@@ -960,7 +963,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$ &quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1013,6 +1016,23 @@
     <font>
       <sz val="12"/>
       <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1090,7 +1110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1223,6 +1243,8 @@
     <xf numFmtId="4" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1729,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1801,7 +1823,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>10</v>
@@ -1837,21 +1859,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="8"/>
     </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="8"/>
     </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
@@ -1859,15 +1881,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="49"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -1875,7 +1898,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
@@ -1883,7 +1906,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
@@ -1891,7 +1914,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
@@ -1899,7 +1922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>28</v>
       </c>
@@ -1907,7 +1930,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>29</v>
       </c>
@@ -1915,7 +1938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>30</v>
       </c>
@@ -1923,21 +1946,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="8"/>
     </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="8"/>
     </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="8"/>
     </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>32</v>
       </c>
@@ -1955,10 +1978,10 @@
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1967,7 +1990,7 @@
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="8"/>
     </row>
@@ -1976,15 +1999,15 @@
       <c r="B37" s="8"/>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
-        <v>3</v>
+      <c r="A38" s="48" t="s">
+        <v>38</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="48" t="s">
         <v>40</v>
       </c>
       <c r="B39" s="8" t="s">
@@ -1993,37 +2016,37 @@
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" s="5"/>
     </row>
@@ -2033,15 +2056,15 @@
     </row>
     <row r="49" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>10</v>
@@ -2053,7 +2076,7 @@
     </row>
     <row r="52" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" s="8"/>
     </row>
@@ -2063,18 +2086,18 @@
     </row>
     <row r="54" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2083,7 +2106,7 @@
     </row>
     <row r="57" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" s="8"/>
     </row>
@@ -2093,47 +2116,47 @@
     </row>
     <row r="59" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>10</v>
@@ -2141,7 +2164,7 @@
     </row>
     <row r="65" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>10</v>
@@ -2149,7 +2172,7 @@
     </row>
     <row r="66" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>10</v>
@@ -2157,7 +2180,7 @@
     </row>
     <row r="67" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B67" s="9" t="s">
         <v>10</v>
@@ -2169,7 +2192,7 @@
     </row>
     <row r="69" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B69" s="8"/>
     </row>
@@ -2179,26 +2202,26 @@
     </row>
     <row r="71" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2207,7 +2230,7 @@
     </row>
     <row r="75" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B75" s="8"/>
     </row>
@@ -2217,42 +2240,42 @@
     </row>
     <row r="77" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B78" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B80" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B81" s="9" t="s">
         <v>89</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2292,79 +2315,79 @@
     <row r="1" spans="1:32" s="2" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:32" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>94</v>
-      </c>
       <c r="F2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>94</v>
-      </c>
       <c r="J2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="L2" s="13" t="s">
-        <v>94</v>
-      </c>
       <c r="N2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="P2" s="13" t="s">
-        <v>94</v>
-      </c>
       <c r="R2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="S2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="T2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="T2" s="13" t="s">
-        <v>94</v>
-      </c>
       <c r="V2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="W2" s="12" t="s">
+      <c r="X2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="X2" s="13" t="s">
-        <v>94</v>
-      </c>
       <c r="Z2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="AA2" s="12" t="s">
+      <c r="AB2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="AB2" s="13" t="s">
-        <v>94</v>
-      </c>
       <c r="AD2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="AE2" s="12" t="s">
+      <c r="AF2" s="13" t="s">
         <v>93</v>
-      </c>
-      <c r="AF2" s="13" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2396,43 +2419,43 @@
     </row>
     <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="C4" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="G4" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="H4" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="J4" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="K4" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="L4" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="N4" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="O4" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="P4" s="18" t="s">
         <v>98</v>
-      </c>
-      <c r="N4" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="P4" s="18" t="s">
-        <v>99</v>
       </c>
       <c r="R4" s="19"/>
       <c r="S4" s="20"/>
@@ -2449,43 +2472,43 @@
     </row>
     <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="C5" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="G5" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="H5" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="J5" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="K5" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="L5" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="N5" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="O5" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="P5" s="18" t="s">
         <v>103</v>
-      </c>
-      <c r="N5" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="O5" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="P5" s="18" t="s">
-        <v>104</v>
       </c>
       <c r="R5" s="22"/>
       <c r="S5" s="17"/>
@@ -2502,43 +2525,43 @@
     </row>
     <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="C6" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="G6" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="H6" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="H6" s="25" t="s">
-        <v>107</v>
-      </c>
       <c r="J6" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P6" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R6" s="23"/>
       <c r="S6" s="24"/>
@@ -2582,7 +2605,7 @@
     </row>
     <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="27"/>
@@ -2638,43 +2661,43 @@
     </row>
     <row r="10" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>110</v>
-      </c>
       <c r="C10" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="G10" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="J10" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="F10" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="17" t="s">
+      <c r="K10" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="N10" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="J10" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="L10" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="N10" s="30" t="s">
-        <v>112</v>
-      </c>
       <c r="O10" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R10" s="29"/>
       <c r="S10" s="17"/>
@@ -2691,43 +2714,43 @@
     </row>
     <row r="11" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="C11" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>115</v>
-      </c>
       <c r="G11" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N11" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R11" s="29"/>
       <c r="S11" s="17"/>
@@ -2744,43 +2767,43 @@
     </row>
     <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="C12" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="F12" s="32" t="s">
-        <v>118</v>
-      </c>
       <c r="G12" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J12" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K12" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L12" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N12" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O12" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P12" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R12" s="31"/>
       <c r="S12" s="24"/>
@@ -2824,7 +2847,7 @@
     </row>
     <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B14" s="29"/>
       <c r="C14" s="36"/>
@@ -2880,43 +2903,43 @@
     </row>
     <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="C16" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="D16" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="F16" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="G16" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="H16" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="H16" s="18" t="s">
-        <v>126</v>
-      </c>
       <c r="J16" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="K16" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="K16" s="17" t="s">
+      <c r="L16" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="L16" s="18" t="s">
-        <v>126</v>
-      </c>
       <c r="N16" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="O16" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="O16" s="17" t="s">
+      <c r="P16" s="18" t="s">
         <v>125</v>
-      </c>
-      <c r="P16" s="18" t="s">
-        <v>126</v>
       </c>
       <c r="R16" s="38"/>
       <c r="S16" s="17"/>
@@ -2933,43 +2956,43 @@
     </row>
     <row r="17" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="B17" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" s="36" t="s">
-        <v>128</v>
-      </c>
       <c r="D17" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="G17" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="H17" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="H17" s="18" t="s">
-        <v>132</v>
-      </c>
       <c r="J17" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="K17" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="K17" s="17" t="s">
+      <c r="L17" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="L17" s="18" t="s">
-        <v>132</v>
-      </c>
       <c r="N17" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="O17" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="O17" s="17" t="s">
+      <c r="P17" s="18" t="s">
         <v>131</v>
-      </c>
-      <c r="P17" s="18" t="s">
-        <v>132</v>
       </c>
       <c r="R17" s="29"/>
       <c r="S17" s="36"/>
@@ -2986,43 +3009,43 @@
     </row>
     <row r="18" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="B18" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="C18" s="40" t="s">
+      <c r="D18" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="F18" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="F18" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="G18" s="24" t="s">
-        <v>136</v>
-      </c>
       <c r="H18" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="J18" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="J18" s="32" t="s">
-        <v>103</v>
-      </c>
       <c r="K18" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L18" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="N18" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="N18" s="32" t="s">
-        <v>103</v>
-      </c>
       <c r="O18" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P18" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="R18" s="39"/>
       <c r="S18" s="40"/>
@@ -3066,7 +3089,7 @@
     </row>
     <row r="20" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B20" s="42"/>
       <c r="C20" s="43"/>
@@ -3122,43 +3145,43 @@
     </row>
     <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J22" s="30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L22" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N22" s="30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O22" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P22" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R22" s="29"/>
       <c r="S22" s="17"/>
@@ -3175,43 +3198,43 @@
     </row>
     <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J23" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L23" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N23" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P23" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R23" s="29"/>
       <c r="S23" s="17"/>
@@ -3228,43 +3251,43 @@
     </row>
     <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="C24" s="36" t="s">
+      <c r="D24" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="F24" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="G24" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="F24" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="G24" s="17" t="s">
+      <c r="H24" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="H24" s="18" t="s">
-        <v>144</v>
-      </c>
       <c r="J24" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K24" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="L24" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="L24" s="18" t="s">
-        <v>144</v>
-      </c>
       <c r="N24" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O24" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="P24" s="18" t="s">
         <v>143</v>
-      </c>
-      <c r="P24" s="18" t="s">
-        <v>144</v>
       </c>
       <c r="R24" s="29"/>
       <c r="S24" s="36"/>
@@ -3281,43 +3304,43 @@
     </row>
     <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="D25" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="F25" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="H25" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="D25" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="F25" s="30" t="s">
+      <c r="J25" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="K25" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="G25" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="H25" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="J25" s="30" t="s">
+      <c r="L25" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="N25" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="O25" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="K25" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="L25" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="N25" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="O25" s="17" t="s">
-        <v>142</v>
-      </c>
       <c r="P25" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R25" s="29"/>
       <c r="S25" s="36"/>
@@ -3334,43 +3357,43 @@
     </row>
     <row r="26" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="B26" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="D26" s="37" t="s">
+      <c r="F26" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H26" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="F26" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="G26" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>150</v>
-      </c>
       <c r="J26" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L26" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N26" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P26" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R26" s="38"/>
       <c r="S26" s="17"/>
@@ -3387,43 +3410,43 @@
     </row>
     <row r="27" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="B27" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="D27" s="37" t="s">
+      <c r="F27" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H27" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="F27" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="H27" s="18" t="s">
-        <v>153</v>
-      </c>
       <c r="J27" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K27" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L27" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N27" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O27" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P27" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R27" s="38"/>
       <c r="S27" s="17"/>
@@ -3440,43 +3463,43 @@
     </row>
     <row r="28" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="B28" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C28" s="36" t="s">
+      <c r="D28" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="F28" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="D28" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="F28" s="30" t="s">
+      <c r="G28" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="H28" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="G28" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="H28" s="18" t="s">
-        <v>157</v>
-      </c>
       <c r="J28" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="L28" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="K28" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="L28" s="18" t="s">
-        <v>157</v>
-      </c>
       <c r="N28" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="O28" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="P28" s="18" t="s">
         <v>156</v>
-      </c>
-      <c r="O28" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="P28" s="18" t="s">
-        <v>157</v>
       </c>
       <c r="R28" s="29"/>
       <c r="S28" s="36"/>
@@ -3493,43 +3516,43 @@
     </row>
     <row r="29" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C29" s="43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D29" s="44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J29" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K29" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L29" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N29" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O29" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P29" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R29" s="42"/>
       <c r="S29" s="43"/>
@@ -3546,43 +3569,43 @@
     </row>
     <row r="30" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C30" s="43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D30" s="44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J30" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L30" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N30" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O30" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P30" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R30" s="42"/>
       <c r="S30" s="43"/>
@@ -3599,43 +3622,43 @@
     </row>
     <row r="31" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B31" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C31" s="43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D31" s="44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J31" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K31" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L31" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N31" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O31" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P31" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R31" s="42"/>
       <c r="S31" s="43"/>
@@ -3652,43 +3675,43 @@
     </row>
     <row r="32" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B32" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C32" s="43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D32" s="44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J32" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K32" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L32" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N32" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O32" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P32" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R32" s="42"/>
       <c r="S32" s="43"/>
@@ -3705,43 +3728,43 @@
     </row>
     <row r="33" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C33" s="43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D33" s="44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J33" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K33" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L33" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N33" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O33" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P33" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R33" s="42"/>
       <c r="S33" s="43"/>
@@ -3758,43 +3781,43 @@
     </row>
     <row r="34" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="F34" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="H34" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="B34" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="C34" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="D34" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="F34" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="H34" s="18" t="s">
-        <v>164</v>
-      </c>
       <c r="J34" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L34" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N34" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O34" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P34" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R34" s="29"/>
       <c r="S34" s="36"/>
@@ -3811,43 +3834,43 @@
     </row>
     <row r="35" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="D35" s="41" t="s">
         <v>165</v>
       </c>
-      <c r="B35" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="C35" s="40" t="s">
-        <v>131</v>
-      </c>
-      <c r="D35" s="41" t="s">
+      <c r="F35" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="G35" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H35" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="F35" s="32" t="s">
+      <c r="J35" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="K35" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="G35" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="H35" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="J35" s="32" t="s">
+      <c r="L35" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="N35" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="O35" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="K35" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="L35" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="N35" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="O35" s="24" t="s">
-        <v>126</v>
-      </c>
       <c r="P35" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R35" s="31"/>
       <c r="S35" s="40"/>
@@ -3891,7 +3914,7 @@
     </row>
     <row r="37" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B37" s="29"/>
       <c r="C37" s="36"/>
@@ -3947,43 +3970,43 @@
     </row>
     <row r="39" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="F39" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="H39" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="B39" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="C39" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="D39" s="37" t="s">
-        <v>144</v>
-      </c>
-      <c r="F39" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="H39" s="18" t="s">
-        <v>170</v>
-      </c>
       <c r="J39" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K39" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L39" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N39" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O39" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P39" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R39" s="29"/>
       <c r="S39" s="36"/>
@@ -4000,43 +4023,43 @@
     </row>
     <row r="40" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="D40" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="F40" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="H40" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="B40" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="C40" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="D40" s="37" t="s">
-        <v>147</v>
-      </c>
-      <c r="F40" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="H40" s="18" t="s">
-        <v>172</v>
-      </c>
       <c r="J40" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K40" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L40" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N40" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O40" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P40" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R40" s="29"/>
       <c r="S40" s="36"/>
@@ -4053,43 +4076,43 @@
     </row>
     <row r="41" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="B41" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="C41" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="D41" s="37" t="s">
+      <c r="F41" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G41" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="F41" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="G41" s="17" t="s">
+      <c r="H41" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="H41" s="18" t="s">
-        <v>176</v>
-      </c>
       <c r="J41" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K41" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L41" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="L41" s="18" t="s">
-        <v>176</v>
-      </c>
       <c r="N41" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O41" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="P41" s="18" t="s">
         <v>175</v>
-      </c>
-      <c r="P41" s="18" t="s">
-        <v>176</v>
       </c>
       <c r="R41" s="29"/>
       <c r="S41" s="36"/>
@@ -4106,43 +4129,43 @@
     </row>
     <row r="42" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="D42" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="F42" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="H42" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="B42" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="C42" s="36" t="s">
+      <c r="J42" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="D42" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="F42" s="30" t="s">
+      <c r="K42" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="G42" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="H42" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="J42" s="30" t="s">
+      <c r="L42" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="N42" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="O42" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="K42" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="L42" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="N42" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="O42" s="17" t="s">
-        <v>144</v>
-      </c>
       <c r="P42" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R42" s="29"/>
       <c r="S42" s="36"/>
@@ -4159,43 +4182,43 @@
     </row>
     <row r="43" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B43" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C43" s="43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D43" s="44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F43" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J43" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K43" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L43" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N43" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O43" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P43" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R43" s="42"/>
       <c r="S43" s="43"/>
@@ -4212,43 +4235,43 @@
     </row>
     <row r="44" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B44" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C44" s="43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D44" s="44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F44" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J44" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K44" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L44" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N44" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O44" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P44" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R44" s="42"/>
       <c r="S44" s="43"/>
@@ -4265,43 +4288,43 @@
     </row>
     <row r="45" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B45" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C45" s="43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D45" s="44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F45" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J45" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K45" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L45" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N45" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O45" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P45" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R45" s="42"/>
       <c r="S45" s="43"/>
@@ -4318,43 +4341,43 @@
     </row>
     <row r="46" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C46" s="43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D46" s="44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F46" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J46" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K46" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L46" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N46" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O46" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P46" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R46" s="42"/>
       <c r="S46" s="43"/>
@@ -4371,43 +4394,43 @@
     </row>
     <row r="47" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B47" s="45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C47" s="46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D47" s="47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F47" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H47" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J47" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K47" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L47" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N47" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O47" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P47" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R47" s="45"/>
       <c r="S47" s="46"/>
@@ -4466,7 +4489,7 @@
     </row>
     <row r="50" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F50"/>
       <c r="G50"/>
@@ -4509,7 +4532,7 @@
     </row>
     <row r="52" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F52"/>
       <c r="G52"/>
@@ -4553,43 +4576,43 @@
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B54" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="B54" s="42" t="s">
+      <c r="C54" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="D54" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="F54" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="C54" s="43" t="s">
+      <c r="G54" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D54" s="44" t="s">
+      <c r="H54" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="F54" s="42" t="s">
+      <c r="J54" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="G54" s="43" t="s">
+      <c r="K54" s="43" t="s">
         <v>187</v>
       </c>
-      <c r="H54" s="44" t="s">
+      <c r="L54" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="J54" s="42" t="s">
+      <c r="N54" s="42" t="s">
         <v>188</v>
       </c>
-      <c r="K54" s="43" t="s">
+      <c r="O54" s="43" t="s">
         <v>188</v>
       </c>
-      <c r="L54" s="44" t="s">
+      <c r="P54" s="44" t="s">
         <v>188</v>
-      </c>
-      <c r="N54" s="42" t="s">
-        <v>189</v>
-      </c>
-      <c r="O54" s="43" t="s">
-        <v>189</v>
-      </c>
-      <c r="P54" s="44" t="s">
-        <v>189</v>
       </c>
       <c r="R54" s="42"/>
       <c r="S54" s="43"/>
@@ -4606,43 +4629,43 @@
     </row>
     <row r="55" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B55" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C55" s="46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D55" s="47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F55" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G55" s="46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H55" s="47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J55" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K55" s="46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L55" s="47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N55" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O55" s="46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P55" s="47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R55" s="45"/>
       <c r="S55" s="46"/>
@@ -4686,7 +4709,7 @@
     </row>
     <row r="57" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57" s="42"/>
       <c r="C57" s="43"/>
@@ -4742,43 +4765,43 @@
     </row>
     <row r="59" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B59" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="B59" s="42" t="s">
+      <c r="C59" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="D59" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F59" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="C59" s="43" t="s">
+      <c r="G59" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="D59" s="44" t="s">
+      <c r="H59" s="44" t="s">
         <v>192</v>
       </c>
-      <c r="F59" s="42" t="s">
+      <c r="J59" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="G59" s="43" t="s">
+      <c r="K59" s="43" t="s">
         <v>193</v>
       </c>
-      <c r="H59" s="44" t="s">
+      <c r="L59" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="J59" s="42" t="s">
+      <c r="N59" s="42" t="s">
         <v>194</v>
       </c>
-      <c r="K59" s="43" t="s">
+      <c r="O59" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="L59" s="44" t="s">
+      <c r="P59" s="44" t="s">
         <v>194</v>
-      </c>
-      <c r="N59" s="42" t="s">
-        <v>195</v>
-      </c>
-      <c r="O59" s="43" t="s">
-        <v>195</v>
-      </c>
-      <c r="P59" s="44" t="s">
-        <v>195</v>
       </c>
       <c r="R59" s="42"/>
       <c r="S59" s="43"/>
@@ -4795,43 +4818,43 @@
     </row>
     <row r="60" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B60" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="B60" s="45" t="s">
+      <c r="C60" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="D60" s="47" t="s">
+        <v>196</v>
+      </c>
+      <c r="F60" s="45" t="s">
         <v>197</v>
       </c>
-      <c r="C60" s="46" t="s">
+      <c r="G60" s="46" t="s">
         <v>197</v>
       </c>
-      <c r="D60" s="47" t="s">
+      <c r="H60" s="47" t="s">
         <v>197</v>
       </c>
-      <c r="F60" s="45" t="s">
+      <c r="J60" s="45" t="s">
         <v>198</v>
       </c>
-      <c r="G60" s="46" t="s">
+      <c r="K60" s="46" t="s">
         <v>198</v>
       </c>
-      <c r="H60" s="47" t="s">
+      <c r="L60" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="J60" s="45" t="s">
+      <c r="N60" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="K60" s="46" t="s">
+      <c r="O60" s="46" t="s">
         <v>199</v>
       </c>
-      <c r="L60" s="47" t="s">
+      <c r="P60" s="47" t="s">
         <v>199</v>
-      </c>
-      <c r="N60" s="45" t="s">
-        <v>200</v>
-      </c>
-      <c r="O60" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="P60" s="47" t="s">
-        <v>200</v>
       </c>
       <c r="R60" s="45"/>
       <c r="S60" s="46"/>
@@ -4875,7 +4898,7 @@
     </row>
     <row r="62" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B62" s="42"/>
       <c r="C62" s="43"/>
@@ -4931,43 +4954,43 @@
     </row>
     <row r="64" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B64" s="42" t="s">
         <v>201</v>
       </c>
-      <c r="B64" s="42" t="s">
+      <c r="C64" s="43" t="s">
+        <v>201</v>
+      </c>
+      <c r="D64" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="F64" s="42" t="s">
         <v>202</v>
       </c>
-      <c r="C64" s="43" t="s">
+      <c r="G64" s="43" t="s">
         <v>202</v>
       </c>
-      <c r="D64" s="44" t="s">
+      <c r="H64" s="44" t="s">
         <v>202</v>
       </c>
-      <c r="F64" s="42" t="s">
+      <c r="J64" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="G64" s="43" t="s">
+      <c r="K64" s="43" t="s">
         <v>203</v>
       </c>
-      <c r="H64" s="44" t="s">
+      <c r="L64" s="44" t="s">
         <v>203</v>
       </c>
-      <c r="J64" s="42" t="s">
+      <c r="N64" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="K64" s="43" t="s">
+      <c r="O64" s="43" t="s">
         <v>204</v>
       </c>
-      <c r="L64" s="44" t="s">
+      <c r="P64" s="44" t="s">
         <v>204</v>
-      </c>
-      <c r="N64" s="42" t="s">
-        <v>205</v>
-      </c>
-      <c r="O64" s="43" t="s">
-        <v>205</v>
-      </c>
-      <c r="P64" s="44" t="s">
-        <v>205</v>
       </c>
       <c r="R64" s="42"/>
       <c r="S64" s="43"/>
@@ -4984,43 +5007,43 @@
     </row>
     <row r="65" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B65" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="B65" s="42" t="s">
+      <c r="C65" s="43" t="s">
+        <v>206</v>
+      </c>
+      <c r="D65" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="F65" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="C65" s="43" t="s">
+      <c r="G65" s="43" t="s">
         <v>207</v>
       </c>
-      <c r="D65" s="44" t="s">
+      <c r="H65" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="F65" s="42" t="s">
+      <c r="J65" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="G65" s="43" t="s">
+      <c r="K65" s="43" t="s">
         <v>208</v>
       </c>
-      <c r="H65" s="44" t="s">
+      <c r="L65" s="44" t="s">
         <v>208</v>
       </c>
-      <c r="J65" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="K65" s="43" t="s">
-        <v>209</v>
-      </c>
-      <c r="L65" s="44" t="s">
-        <v>209</v>
-      </c>
       <c r="N65" s="42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O65" s="43" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P65" s="44" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="R65" s="42"/>
       <c r="S65" s="43"/>
@@ -5037,43 +5060,43 @@
     </row>
     <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B66" s="42" t="s">
         <v>210</v>
       </c>
-      <c r="B66" s="42" t="s">
+      <c r="C66" s="43" t="s">
+        <v>210</v>
+      </c>
+      <c r="D66" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="F66" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="C66" s="43" t="s">
+      <c r="G66" s="43" t="s">
         <v>211</v>
       </c>
-      <c r="D66" s="44" t="s">
+      <c r="H66" s="44" t="s">
         <v>211</v>
       </c>
-      <c r="F66" s="42" t="s">
+      <c r="J66" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="G66" s="43" t="s">
+      <c r="K66" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="H66" s="44" t="s">
+      <c r="L66" s="44" t="s">
         <v>212</v>
       </c>
-      <c r="J66" s="42" t="s">
+      <c r="N66" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="K66" s="43" t="s">
+      <c r="O66" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="L66" s="44" t="s">
+      <c r="P66" s="44" t="s">
         <v>213</v>
-      </c>
-      <c r="N66" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="O66" s="43" t="s">
-        <v>214</v>
-      </c>
-      <c r="P66" s="44" t="s">
-        <v>214</v>
       </c>
       <c r="R66" s="42"/>
       <c r="S66" s="43"/>
@@ -5090,43 +5113,43 @@
     </row>
     <row r="67" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B67" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="B67" s="42" t="s">
+      <c r="C67" s="43" t="s">
+        <v>215</v>
+      </c>
+      <c r="D67" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="F67" s="42" t="s">
         <v>216</v>
       </c>
-      <c r="C67" s="43" t="s">
+      <c r="G67" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="D67" s="44" t="s">
+      <c r="H67" s="44" t="s">
         <v>216</v>
       </c>
-      <c r="F67" s="42" t="s">
+      <c r="J67" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="G67" s="43" t="s">
+      <c r="K67" s="43" t="s">
         <v>217</v>
       </c>
-      <c r="H67" s="44" t="s">
+      <c r="L67" s="44" t="s">
         <v>217</v>
       </c>
-      <c r="J67" s="42" t="s">
-        <v>218</v>
-      </c>
-      <c r="K67" s="43" t="s">
-        <v>218</v>
-      </c>
-      <c r="L67" s="44" t="s">
-        <v>218</v>
-      </c>
       <c r="N67" s="42" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O67" s="43" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P67" s="44" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R67" s="42"/>
       <c r="S67" s="43"/>
@@ -5143,43 +5166,43 @@
     </row>
     <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B68" s="42" t="s">
         <v>219</v>
       </c>
-      <c r="B68" s="42" t="s">
+      <c r="C68" s="43" t="s">
+        <v>219</v>
+      </c>
+      <c r="D68" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="F68" s="42" t="s">
         <v>220</v>
       </c>
-      <c r="C68" s="43" t="s">
+      <c r="G68" s="43" t="s">
         <v>220</v>
       </c>
-      <c r="D68" s="44" t="s">
+      <c r="H68" s="44" t="s">
         <v>220</v>
       </c>
-      <c r="F68" s="42" t="s">
+      <c r="J68" s="42" t="s">
         <v>221</v>
       </c>
-      <c r="G68" s="43" t="s">
+      <c r="K68" s="43" t="s">
         <v>221</v>
       </c>
-      <c r="H68" s="44" t="s">
+      <c r="L68" s="44" t="s">
         <v>221</v>
       </c>
-      <c r="J68" s="42" t="s">
+      <c r="N68" s="42" t="s">
         <v>222</v>
       </c>
-      <c r="K68" s="43" t="s">
+      <c r="O68" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="L68" s="44" t="s">
+      <c r="P68" s="44" t="s">
         <v>222</v>
-      </c>
-      <c r="N68" s="42" t="s">
-        <v>223</v>
-      </c>
-      <c r="O68" s="43" t="s">
-        <v>223</v>
-      </c>
-      <c r="P68" s="44" t="s">
-        <v>223</v>
       </c>
       <c r="R68" s="42"/>
       <c r="S68" s="43"/>
@@ -5196,43 +5219,43 @@
     </row>
     <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B69" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C69" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D69" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F69" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G69" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H69" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J69" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K69" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L69" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N69" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O69" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P69" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R69" s="42"/>
       <c r="S69" s="43"/>
@@ -5249,43 +5272,43 @@
     </row>
     <row r="70" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B70" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C70" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D70" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F70" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G70" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H70" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J70" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K70" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L70" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N70" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O70" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P70" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R70" s="42"/>
       <c r="S70" s="43"/>
@@ -5302,43 +5325,43 @@
     </row>
     <row r="71" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B71" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C71" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D71" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F71" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G71" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H71" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J71" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K71" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L71" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N71" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O71" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P71" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R71" s="42"/>
       <c r="S71" s="43"/>
@@ -5355,43 +5378,43 @@
     </row>
     <row r="72" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B72" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C72" s="46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D72" s="47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F72" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G72" s="46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H72" s="47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J72" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K72" s="46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L72" s="47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N72" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O72" s="46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P72" s="47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R72" s="45"/>
       <c r="S72" s="46"/>
@@ -5435,7 +5458,7 @@
     </row>
     <row r="74" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" s="42"/>
       <c r="C74" s="43"/>
@@ -5491,43 +5514,43 @@
     </row>
     <row r="76" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B76" s="42" t="s">
         <v>228</v>
       </c>
-      <c r="B76" s="42" t="s">
+      <c r="C76" s="43" t="s">
+        <v>228</v>
+      </c>
+      <c r="D76" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="F76" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="C76" s="43" t="s">
+      <c r="G76" s="43" t="s">
         <v>229</v>
       </c>
-      <c r="D76" s="44" t="s">
+      <c r="H76" s="44" t="s">
         <v>229</v>
       </c>
-      <c r="F76" s="42" t="s">
+      <c r="J76" s="42" t="s">
         <v>230</v>
       </c>
-      <c r="G76" s="43" t="s">
+      <c r="K76" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="H76" s="44" t="s">
+      <c r="L76" s="44" t="s">
         <v>230</v>
       </c>
-      <c r="J76" s="42" t="s">
+      <c r="N76" s="42" t="s">
         <v>231</v>
       </c>
-      <c r="K76" s="43" t="s">
+      <c r="O76" s="43" t="s">
         <v>231</v>
       </c>
-      <c r="L76" s="44" t="s">
+      <c r="P76" s="44" t="s">
         <v>231</v>
-      </c>
-      <c r="N76" s="42" t="s">
-        <v>232</v>
-      </c>
-      <c r="O76" s="43" t="s">
-        <v>232</v>
-      </c>
-      <c r="P76" s="44" t="s">
-        <v>232</v>
       </c>
       <c r="R76" s="42"/>
       <c r="S76" s="43"/>
@@ -5544,43 +5567,43 @@
     </row>
     <row r="77" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B77" s="42" t="s">
         <v>233</v>
       </c>
-      <c r="B77" s="42" t="s">
+      <c r="C77" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="D77" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="F77" s="42" t="s">
         <v>234</v>
       </c>
-      <c r="C77" s="43" t="s">
+      <c r="G77" s="43" t="s">
         <v>234</v>
       </c>
-      <c r="D77" s="44" t="s">
+      <c r="H77" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="F77" s="42" t="s">
+      <c r="J77" s="42" t="s">
         <v>235</v>
       </c>
-      <c r="G77" s="43" t="s">
+      <c r="K77" s="43" t="s">
         <v>235</v>
       </c>
-      <c r="H77" s="44" t="s">
+      <c r="L77" s="44" t="s">
         <v>235</v>
       </c>
-      <c r="J77" s="42" t="s">
+      <c r="N77" s="42" t="s">
         <v>236</v>
       </c>
-      <c r="K77" s="43" t="s">
+      <c r="O77" s="43" t="s">
         <v>236</v>
       </c>
-      <c r="L77" s="44" t="s">
+      <c r="P77" s="44" t="s">
         <v>236</v>
-      </c>
-      <c r="N77" s="42" t="s">
-        <v>237</v>
-      </c>
-      <c r="O77" s="43" t="s">
-        <v>237</v>
-      </c>
-      <c r="P77" s="44" t="s">
-        <v>237</v>
       </c>
       <c r="R77" s="42"/>
       <c r="S77" s="43"/>
@@ -5597,43 +5620,43 @@
     </row>
     <row r="78" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B78" s="45" t="s">
         <v>238</v>
       </c>
-      <c r="B78" s="45" t="s">
+      <c r="C78" s="46" t="s">
+        <v>238</v>
+      </c>
+      <c r="D78" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="F78" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="C78" s="46" t="s">
+      <c r="G78" s="46" t="s">
         <v>239</v>
       </c>
-      <c r="D78" s="47" t="s">
+      <c r="H78" s="47" t="s">
         <v>239</v>
       </c>
-      <c r="F78" s="45" t="s">
+      <c r="J78" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="G78" s="46" t="s">
+      <c r="K78" s="46" t="s">
         <v>240</v>
       </c>
-      <c r="H78" s="47" t="s">
+      <c r="L78" s="47" t="s">
         <v>240</v>
       </c>
-      <c r="J78" s="45" t="s">
+      <c r="N78" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="K78" s="46" t="s">
+      <c r="O78" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="L78" s="47" t="s">
+      <c r="P78" s="47" t="s">
         <v>241</v>
-      </c>
-      <c r="N78" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="O78" s="46" t="s">
-        <v>242</v>
-      </c>
-      <c r="P78" s="47" t="s">
-        <v>242</v>
       </c>
       <c r="R78" s="45"/>
       <c r="S78" s="46"/>
@@ -5677,7 +5700,7 @@
     </row>
     <row r="80" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B80" s="42"/>
       <c r="C80" s="43"/>
@@ -5733,43 +5756,43 @@
     </row>
     <row r="82" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B82" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="B82" s="42" t="s">
+      <c r="C82" s="43" t="s">
+        <v>243</v>
+      </c>
+      <c r="D82" s="44" t="s">
+        <v>243</v>
+      </c>
+      <c r="F82" s="42" t="s">
         <v>244</v>
       </c>
-      <c r="C82" s="43" t="s">
+      <c r="G82" s="43" t="s">
         <v>244</v>
       </c>
-      <c r="D82" s="44" t="s">
+      <c r="H82" s="44" t="s">
         <v>244</v>
       </c>
-      <c r="F82" s="42" t="s">
+      <c r="J82" s="42" t="s">
         <v>245</v>
       </c>
-      <c r="G82" s="43" t="s">
+      <c r="K82" s="43" t="s">
         <v>245</v>
       </c>
-      <c r="H82" s="44" t="s">
+      <c r="L82" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="J82" s="42" t="s">
+      <c r="N82" s="42" t="s">
         <v>246</v>
       </c>
-      <c r="K82" s="43" t="s">
+      <c r="O82" s="43" t="s">
         <v>246</v>
       </c>
-      <c r="L82" s="44" t="s">
+      <c r="P82" s="44" t="s">
         <v>246</v>
-      </c>
-      <c r="N82" s="42" t="s">
-        <v>247</v>
-      </c>
-      <c r="O82" s="43" t="s">
-        <v>247</v>
-      </c>
-      <c r="P82" s="44" t="s">
-        <v>247</v>
       </c>
       <c r="R82" s="42"/>
       <c r="S82" s="43"/>
@@ -5786,43 +5809,43 @@
     </row>
     <row r="83" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B83" s="42" t="s">
         <v>248</v>
       </c>
-      <c r="B83" s="42" t="s">
+      <c r="C83" s="43" t="s">
+        <v>248</v>
+      </c>
+      <c r="D83" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="F83" s="42" t="s">
         <v>249</v>
       </c>
-      <c r="C83" s="43" t="s">
+      <c r="G83" s="43" t="s">
         <v>249</v>
       </c>
-      <c r="D83" s="44" t="s">
+      <c r="H83" s="44" t="s">
         <v>249</v>
       </c>
-      <c r="F83" s="42" t="s">
+      <c r="J83" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="G83" s="43" t="s">
+      <c r="K83" s="43" t="s">
         <v>250</v>
       </c>
-      <c r="H83" s="44" t="s">
+      <c r="L83" s="44" t="s">
         <v>250</v>
       </c>
-      <c r="J83" s="42" t="s">
+      <c r="N83" s="42" t="s">
         <v>251</v>
       </c>
-      <c r="K83" s="43" t="s">
+      <c r="O83" s="43" t="s">
         <v>251</v>
       </c>
-      <c r="L83" s="44" t="s">
+      <c r="P83" s="44" t="s">
         <v>251</v>
-      </c>
-      <c r="N83" s="42" t="s">
-        <v>252</v>
-      </c>
-      <c r="O83" s="43" t="s">
-        <v>252</v>
-      </c>
-      <c r="P83" s="44" t="s">
-        <v>252</v>
       </c>
       <c r="R83" s="42"/>
       <c r="S83" s="43"/>
@@ -5839,43 +5862,43 @@
     </row>
     <row r="84" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B84" s="42" t="s">
         <v>253</v>
       </c>
-      <c r="B84" s="42" t="s">
+      <c r="C84" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="D84" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="F84" s="42" t="s">
         <v>254</v>
       </c>
-      <c r="C84" s="43" t="s">
+      <c r="G84" s="43" t="s">
         <v>254</v>
       </c>
-      <c r="D84" s="44" t="s">
+      <c r="H84" s="44" t="s">
         <v>254</v>
       </c>
-      <c r="F84" s="42" t="s">
+      <c r="J84" s="42" t="s">
         <v>255</v>
       </c>
-      <c r="G84" s="43" t="s">
+      <c r="K84" s="43" t="s">
         <v>255</v>
       </c>
-      <c r="H84" s="44" t="s">
+      <c r="L84" s="44" t="s">
         <v>255</v>
       </c>
-      <c r="J84" s="42" t="s">
+      <c r="N84" s="42" t="s">
         <v>256</v>
       </c>
-      <c r="K84" s="43" t="s">
+      <c r="O84" s="43" t="s">
         <v>256</v>
       </c>
-      <c r="L84" s="44" t="s">
+      <c r="P84" s="44" t="s">
         <v>256</v>
-      </c>
-      <c r="N84" s="42" t="s">
-        <v>257</v>
-      </c>
-      <c r="O84" s="43" t="s">
-        <v>257</v>
-      </c>
-      <c r="P84" s="44" t="s">
-        <v>257</v>
       </c>
       <c r="R84" s="42"/>
       <c r="S84" s="43"/>
@@ -5892,43 +5915,43 @@
     </row>
     <row r="85" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B85" s="42" t="s">
         <v>258</v>
       </c>
-      <c r="B85" s="42" t="s">
+      <c r="C85" s="43" t="s">
+        <v>258</v>
+      </c>
+      <c r="D85" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="F85" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="C85" s="43" t="s">
+      <c r="G85" s="43" t="s">
         <v>259</v>
       </c>
-      <c r="D85" s="44" t="s">
+      <c r="H85" s="44" t="s">
         <v>259</v>
       </c>
-      <c r="F85" s="42" t="s">
+      <c r="J85" s="42" t="s">
         <v>260</v>
       </c>
-      <c r="G85" s="43" t="s">
+      <c r="K85" s="43" t="s">
         <v>260</v>
       </c>
-      <c r="H85" s="44" t="s">
+      <c r="L85" s="44" t="s">
         <v>260</v>
       </c>
-      <c r="J85" s="42" t="s">
+      <c r="N85" s="42" t="s">
         <v>261</v>
       </c>
-      <c r="K85" s="43" t="s">
+      <c r="O85" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="L85" s="44" t="s">
+      <c r="P85" s="44" t="s">
         <v>261</v>
-      </c>
-      <c r="N85" s="42" t="s">
-        <v>262</v>
-      </c>
-      <c r="O85" s="43" t="s">
-        <v>262</v>
-      </c>
-      <c r="P85" s="44" t="s">
-        <v>262</v>
       </c>
       <c r="R85" s="42"/>
       <c r="S85" s="43"/>
@@ -5945,43 +5968,43 @@
     </row>
     <row r="86" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B86" s="45" t="s">
         <v>263</v>
       </c>
-      <c r="B86" s="45" t="s">
+      <c r="C86" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="D86" s="47" t="s">
+        <v>263</v>
+      </c>
+      <c r="F86" s="45" t="s">
         <v>264</v>
       </c>
-      <c r="C86" s="46" t="s">
+      <c r="G86" s="46" t="s">
         <v>264</v>
       </c>
-      <c r="D86" s="47" t="s">
+      <c r="H86" s="47" t="s">
         <v>264</v>
       </c>
-      <c r="F86" s="45" t="s">
+      <c r="J86" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="G86" s="46" t="s">
+      <c r="K86" s="46" t="s">
         <v>265</v>
       </c>
-      <c r="H86" s="47" t="s">
+      <c r="L86" s="47" t="s">
         <v>265</v>
       </c>
-      <c r="J86" s="45" t="s">
+      <c r="N86" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="K86" s="46" t="s">
+      <c r="O86" s="46" t="s">
         <v>266</v>
       </c>
-      <c r="L86" s="47" t="s">
+      <c r="P86" s="47" t="s">
         <v>266</v>
-      </c>
-      <c r="N86" s="45" t="s">
-        <v>267</v>
-      </c>
-      <c r="O86" s="46" t="s">
-        <v>267</v>
-      </c>
-      <c r="P86" s="47" t="s">
-        <v>267</v>
       </c>
       <c r="R86" s="45"/>
       <c r="S86" s="46"/>
@@ -6024,7 +6047,7 @@
     </row>
     <row r="88" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="43"/>
@@ -6053,43 +6076,43 @@
     </row>
     <row r="89" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B89" s="42" t="s">
         <v>269</v>
       </c>
-      <c r="B89" s="42" t="s">
+      <c r="C89" s="43" t="s">
         <v>270</v>
       </c>
-      <c r="C89" s="43" t="s">
+      <c r="D89" s="44" t="s">
         <v>271</v>
       </c>
-      <c r="D89" s="44" t="s">
+      <c r="F89" s="42" t="s">
         <v>272</v>
       </c>
-      <c r="F89" s="42" t="s">
+      <c r="G89" s="43" t="s">
         <v>273</v>
       </c>
-      <c r="G89" s="43" t="s">
+      <c r="H89" s="44" t="s">
         <v>274</v>
       </c>
-      <c r="H89" s="44" t="s">
+      <c r="J89" s="42" t="s">
         <v>275</v>
       </c>
-      <c r="J89" s="42" t="s">
+      <c r="K89" s="43" t="s">
         <v>276</v>
       </c>
-      <c r="K89" s="43" t="s">
+      <c r="L89" s="44" t="s">
         <v>277</v>
       </c>
-      <c r="L89" s="44" t="s">
+      <c r="N89" s="42" t="s">
         <v>278</v>
       </c>
-      <c r="N89" s="42" t="s">
+      <c r="O89" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="O89" s="43" t="s">
+      <c r="P89" s="44" t="s">
         <v>280</v>
-      </c>
-      <c r="P89" s="44" t="s">
-        <v>281</v>
       </c>
       <c r="R89" s="42"/>
       <c r="S89" s="43"/>
@@ -6106,43 +6129,43 @@
     </row>
     <row r="90" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B90" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="C90" s="43" t="s">
         <v>282</v>
       </c>
-      <c r="B90" s="42" t="s">
-        <v>270</v>
-      </c>
-      <c r="C90" s="43" t="s">
+      <c r="D90" s="44" t="s">
         <v>283</v>
       </c>
-      <c r="D90" s="44" t="s">
+      <c r="F90" s="42" t="s">
+        <v>272</v>
+      </c>
+      <c r="G90" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="F90" s="42" t="s">
-        <v>273</v>
-      </c>
-      <c r="G90" s="43" t="s">
+      <c r="H90" s="44" t="s">
         <v>285</v>
       </c>
-      <c r="H90" s="44" t="s">
+      <c r="J90" s="42" t="s">
+        <v>275</v>
+      </c>
+      <c r="K90" s="43" t="s">
         <v>286</v>
       </c>
-      <c r="J90" s="42" t="s">
-        <v>276</v>
-      </c>
-      <c r="K90" s="43" t="s">
+      <c r="L90" s="44" t="s">
         <v>287</v>
       </c>
-      <c r="L90" s="44" t="s">
+      <c r="N90" s="42" t="s">
+        <v>278</v>
+      </c>
+      <c r="O90" s="43" t="s">
         <v>288</v>
       </c>
-      <c r="N90" s="42" t="s">
-        <v>279</v>
-      </c>
-      <c r="O90" s="43" t="s">
+      <c r="P90" s="44" t="s">
         <v>289</v>
-      </c>
-      <c r="P90" s="44" t="s">
-        <v>290</v>
       </c>
       <c r="R90" s="42"/>
       <c r="S90" s="43"/>
@@ -6159,43 +6182,43 @@
     </row>
     <row r="91" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B91" s="42" t="s">
         <v>291</v>
       </c>
-      <c r="B91" s="42" t="s">
+      <c r="C91" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="C91" s="43" t="s">
+      <c r="D91" s="44" t="s">
         <v>293</v>
       </c>
-      <c r="D91" s="44" t="s">
+      <c r="F91" s="42" t="s">
         <v>294</v>
       </c>
-      <c r="F91" s="42" t="s">
+      <c r="G91" s="43" t="s">
         <v>295</v>
       </c>
-      <c r="G91" s="43" t="s">
+      <c r="H91" s="44" t="s">
         <v>296</v>
       </c>
-      <c r="H91" s="44" t="s">
+      <c r="J91" s="42" t="s">
         <v>297</v>
       </c>
-      <c r="J91" s="42" t="s">
+      <c r="K91" s="43" t="s">
         <v>298</v>
       </c>
-      <c r="K91" s="43" t="s">
+      <c r="L91" s="44" t="s">
         <v>299</v>
       </c>
-      <c r="L91" s="44" t="s">
+      <c r="N91" s="42" t="s">
         <v>300</v>
       </c>
-      <c r="N91" s="42" t="s">
+      <c r="O91" s="43" t="s">
         <v>301</v>
       </c>
-      <c r="O91" s="43" t="s">
+      <c r="P91" s="44" t="s">
         <v>302</v>
-      </c>
-      <c r="P91" s="44" t="s">
-        <v>303</v>
       </c>
       <c r="R91" s="42"/>
       <c r="S91" s="43"/>
@@ -6212,43 +6235,43 @@
     </row>
     <row r="92" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B92" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C92" s="43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D92" s="44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F92" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G92" s="43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H92" s="44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J92" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K92" s="43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L92" s="44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N92" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O92" s="43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P92" s="44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R92" s="42"/>
       <c r="S92" s="43"/>
@@ -6265,43 +6288,43 @@
     </row>
     <row r="93" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="B93" s="45" t="s">
         <v>305</v>
       </c>
-      <c r="B93" s="45" t="s">
-        <v>306</v>
-      </c>
       <c r="C93" s="46" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D93" s="47" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F93" s="45" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G93" s="46" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H93" s="47" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J93" s="45" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K93" s="46" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L93" s="47" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="N93" s="45" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="O93" s="46" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P93" s="47" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="R93" s="45"/>
       <c r="S93" s="46"/>

</xml_diff>

<commit_message>
Ajustes na base do dashboard e na leitura da planilha de guarda-chuva
</commit_message>
<xml_diff>
--- a/DashboardModelo1/dadosPlanilha/planilha_saida.xlsx
+++ b/DashboardModelo1/dadosPlanilha/planilha_saida.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sandbox\DashboardCotton\DashboardModelo1\dadosPlanilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44737B50-E7C6-4A83-A36A-FBF369B371A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EBFC05-FC89-4CC5-973A-9ACF7F0155D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -488,9 +488,6 @@
     <t>66</t>
   </si>
   <si>
-    <t>3.7 - Serviços terceirizados - Aluguel de máquinas e outro</t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
@@ -500,21 +497,6 @@
     <t>36</t>
   </si>
   <si>
-    <t>3.7.1 - Serviço terceirizado - Aluguel de máquinas e outro 1 -</t>
-  </si>
-  <si>
-    <t>3.7.2 - Serviço terceirizado - Aluguel de máquinas e outro 2 -</t>
-  </si>
-  <si>
-    <t>3.7.3 - Serviço terceirizado - Aluguel de máquinas e outro 3 -</t>
-  </si>
-  <si>
-    <t>3.7.4 - Serviço terceirizado - Aluguel de máquinas e outro 4 -</t>
-  </si>
-  <si>
-    <t>3.7.5 - Serviço terceirizado - Aluguel de máquinas e outro 5 -</t>
-  </si>
-  <si>
     <t>3.8 - Irrigação (A)</t>
   </si>
   <si>
@@ -563,21 +545,6 @@
     <t>43</t>
   </si>
   <si>
-    <t>4.1.4.1 - Adjuvante / Outros 1 -</t>
-  </si>
-  <si>
-    <t>4.1.4.2 - Adjuvante / Outros 2 -</t>
-  </si>
-  <si>
-    <t>4.1.4.3 - Adjuvante / Outros 3 -</t>
-  </si>
-  <si>
-    <t>4.1.4.4 - Adjuvante / Outros 4 -</t>
-  </si>
-  <si>
-    <t>4.1.4.5 - Adjuvante / Outros 5 -</t>
-  </si>
-  <si>
     <t>CUSTO POR HECTARE</t>
   </si>
   <si>
@@ -954,6 +921,39 @@
   </si>
   <si>
     <t>1.3 Despesas Gerais</t>
+  </si>
+  <si>
+    <t>3.7 - Serviço terceirizado - Aluguel de máquinas e outro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.7.1 - Serviço terceirizado - Aluguel de máquinas e outro 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.7.2 - Serviço terceirizado - Aluguel de máquinas e outro 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.7.3 - Serviço terceirizado - Aluguel de máquinas e outro 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.7.4 - Serviço terceirizado - Aluguel de máquinas e outro 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.7.5 - Serviço terceirizado - Aluguel de máquinas e outro 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.1.4.1 - Adjuvante / Outros 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.1.4.2 - Adjuvante / Outros 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.1.4.3 - Adjuvante / Outros 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.1.4.4 - Adjuvante / Outros 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.1.4.5 - Adjuvante / Outros 5 </t>
   </si>
 </sst>
 </file>
@@ -1751,7 +1751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>10</v>
@@ -1978,7 +1978,7 @@
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>36</v>
@@ -2016,7 +2016,7 @@
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>42</v>
@@ -2297,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AF93"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3463,43 +3463,43 @@
     </row>
     <row r="28" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>153</v>
+        <v>298</v>
       </c>
       <c r="B28" s="29" t="s">
         <v>127</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D28" s="37" t="s">
         <v>131</v>
       </c>
       <c r="F28" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>148</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J28" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K28" s="17" t="s">
         <v>148</v>
       </c>
       <c r="L28" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N28" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O28" s="17" t="s">
         <v>148</v>
       </c>
       <c r="P28" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R28" s="29"/>
       <c r="S28" s="36"/>
@@ -3516,7 +3516,7 @@
     </row>
     <row r="29" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>157</v>
+        <v>299</v>
       </c>
       <c r="B29" s="42" t="s">
         <v>128</v>
@@ -3569,7 +3569,7 @@
     </row>
     <row r="30" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>158</v>
+        <v>300</v>
       </c>
       <c r="B30" s="42" t="s">
         <v>128</v>
@@ -3622,7 +3622,7 @@
     </row>
     <row r="31" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>159</v>
+        <v>301</v>
       </c>
       <c r="B31" s="42" t="s">
         <v>128</v>
@@ -3675,7 +3675,7 @@
     </row>
     <row r="32" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>160</v>
+        <v>302</v>
       </c>
       <c r="B32" s="42" t="s">
         <v>128</v>
@@ -3728,7 +3728,7 @@
     </row>
     <row r="33" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>161</v>
+        <v>303</v>
       </c>
       <c r="B33" s="42" t="s">
         <v>128</v>
@@ -3781,7 +3781,7 @@
     </row>
     <row r="34" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B34" s="29" t="s">
         <v>133</v>
@@ -3793,31 +3793,31 @@
         <v>101</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>151</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="J34" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K34" s="17" t="s">
         <v>151</v>
       </c>
       <c r="L34" s="18" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="N34" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O34" s="17" t="s">
         <v>151</v>
       </c>
       <c r="P34" s="18" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="R34" s="29"/>
       <c r="S34" s="36"/>
@@ -3834,7 +3834,7 @@
     </row>
     <row r="35" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B35" s="31" t="s">
         <v>140</v>
@@ -3843,7 +3843,7 @@
         <v>130</v>
       </c>
       <c r="D35" s="41" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F35" s="32" t="s">
         <v>124</v>
@@ -3852,7 +3852,7 @@
         <v>125</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="J35" s="32" t="s">
         <v>124</v>
@@ -3861,7 +3861,7 @@
         <v>125</v>
       </c>
       <c r="L35" s="25" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="N35" s="32" t="s">
         <v>124</v>
@@ -3870,7 +3870,7 @@
         <v>125</v>
       </c>
       <c r="P35" s="25" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="R35" s="31"/>
       <c r="S35" s="40"/>
@@ -3914,7 +3914,7 @@
     </row>
     <row r="37" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B37" s="29"/>
       <c r="C37" s="36"/>
@@ -3970,10 +3970,10 @@
     </row>
     <row r="39" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C39" s="36" t="s">
         <v>122</v>
@@ -3988,7 +3988,7 @@
         <v>101</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="J39" s="30" t="s">
         <v>135</v>
@@ -3997,7 +3997,7 @@
         <v>101</v>
       </c>
       <c r="L39" s="18" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="N39" s="30" t="s">
         <v>135</v>
@@ -4006,7 +4006,7 @@
         <v>101</v>
       </c>
       <c r="P39" s="18" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="R39" s="29"/>
       <c r="S39" s="36"/>
@@ -4023,10 +4023,10 @@
     </row>
     <row r="40" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C40" s="36" t="s">
         <v>134</v>
@@ -4038,28 +4038,28 @@
         <v>122</v>
       </c>
       <c r="G40" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="H40" s="18" t="s">
         <v>165</v>
-      </c>
-      <c r="H40" s="18" t="s">
-        <v>171</v>
       </c>
       <c r="J40" s="30" t="s">
         <v>122</v>
       </c>
       <c r="K40" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="L40" s="18" t="s">
         <v>165</v>
-      </c>
-      <c r="L40" s="18" t="s">
-        <v>171</v>
       </c>
       <c r="N40" s="30" t="s">
         <v>122</v>
       </c>
       <c r="O40" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="P40" s="18" t="s">
         <v>165</v>
-      </c>
-      <c r="P40" s="18" t="s">
-        <v>171</v>
       </c>
       <c r="R40" s="29"/>
       <c r="S40" s="36"/>
@@ -4076,7 +4076,7 @@
     </row>
     <row r="41" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B41" s="29" t="s">
         <v>124</v>
@@ -4085,34 +4085,34 @@
         <v>142</v>
       </c>
       <c r="D41" s="37" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F41" s="30" t="s">
         <v>134</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="J41" s="30" t="s">
         <v>134</v>
       </c>
       <c r="K41" s="17" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="L41" s="18" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="N41" s="30" t="s">
         <v>134</v>
       </c>
       <c r="O41" s="17" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="P41" s="18" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="R41" s="29"/>
       <c r="S41" s="36"/>
@@ -4129,7 +4129,7 @@
     </row>
     <row r="42" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B42" s="29" t="s">
         <v>130</v>
@@ -4138,7 +4138,7 @@
         <v>141</v>
       </c>
       <c r="D42" s="37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F42" s="30" t="s">
         <v>142</v>
@@ -4147,7 +4147,7 @@
         <v>143</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="J42" s="30" t="s">
         <v>142</v>
@@ -4156,7 +4156,7 @@
         <v>143</v>
       </c>
       <c r="L42" s="18" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="N42" s="30" t="s">
         <v>142</v>
@@ -4165,7 +4165,7 @@
         <v>143</v>
       </c>
       <c r="P42" s="18" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="R42" s="29"/>
       <c r="S42" s="36"/>
@@ -4182,7 +4182,7 @@
     </row>
     <row r="43" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>178</v>
+        <v>304</v>
       </c>
       <c r="B43" s="42" t="s">
         <v>128</v>
@@ -4235,7 +4235,7 @@
     </row>
     <row r="44" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>179</v>
+        <v>305</v>
       </c>
       <c r="B44" s="42" t="s">
         <v>128</v>
@@ -4288,7 +4288,7 @@
     </row>
     <row r="45" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>180</v>
+        <v>306</v>
       </c>
       <c r="B45" s="42" t="s">
         <v>128</v>
@@ -4341,7 +4341,7 @@
     </row>
     <row r="46" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>181</v>
+        <v>307</v>
       </c>
       <c r="B46" s="42" t="s">
         <v>128</v>
@@ -4394,7 +4394,7 @@
     </row>
     <row r="47" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>182</v>
+        <v>308</v>
       </c>
       <c r="B47" s="45" t="s">
         <v>128</v>
@@ -4489,7 +4489,7 @@
     </row>
     <row r="50" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F50"/>
       <c r="G50"/>
@@ -4576,43 +4576,43 @@
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B54" s="42" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C54" s="43" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D54" s="44" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="F54" s="42" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="G54" s="43" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="H54" s="44" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="J54" s="42" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="K54" s="43" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="L54" s="44" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="N54" s="42" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="O54" s="43" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="P54" s="44" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="R54" s="42"/>
       <c r="S54" s="43"/>
@@ -4629,7 +4629,7 @@
     </row>
     <row r="55" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B55" s="45" t="s">
         <v>110</v>
@@ -4765,43 +4765,43 @@
     </row>
     <row r="59" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="B59" s="42" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="C59" s="43" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D59" s="44" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="F59" s="42" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="G59" s="43" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="H59" s="44" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="J59" s="42" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="K59" s="43" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="L59" s="44" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="N59" s="42" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="O59" s="43" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="P59" s="44" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="R59" s="42"/>
       <c r="S59" s="43"/>
@@ -4818,43 +4818,43 @@
     </row>
     <row r="60" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B60" s="45" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="C60" s="46" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="D60" s="47" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="F60" s="45" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="G60" s="46" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="H60" s="47" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="J60" s="45" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="K60" s="46" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="L60" s="47" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="N60" s="45" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="O60" s="46" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="P60" s="47" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="R60" s="45"/>
       <c r="S60" s="46"/>
@@ -4954,43 +4954,43 @@
     </row>
     <row r="64" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B64" s="42" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="C64" s="43" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D64" s="44" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="F64" s="42" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="G64" s="43" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="H64" s="44" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="J64" s="42" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="K64" s="43" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="L64" s="44" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="N64" s="42" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="O64" s="43" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="P64" s="44" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="R64" s="42"/>
       <c r="S64" s="43"/>
@@ -5007,43 +5007,43 @@
     </row>
     <row r="65" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B65" s="42" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C65" s="43" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="D65" s="44" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="F65" s="42" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="G65" s="43" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="H65" s="44" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="J65" s="42" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="K65" s="43" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="L65" s="44" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="N65" s="42" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="O65" s="43" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="P65" s="44" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="R65" s="42"/>
       <c r="S65" s="43"/>
@@ -5060,43 +5060,43 @@
     </row>
     <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="B66" s="42" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C66" s="43" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="D66" s="44" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="F66" s="42" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="G66" s="43" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="H66" s="44" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="J66" s="42" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="K66" s="43" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="L66" s="44" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="N66" s="42" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="O66" s="43" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="P66" s="44" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="R66" s="42"/>
       <c r="S66" s="43"/>
@@ -5113,43 +5113,43 @@
     </row>
     <row r="67" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B67" s="42" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="C67" s="43" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="D67" s="44" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="F67" s="42" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="G67" s="43" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="H67" s="44" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="J67" s="42" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="K67" s="43" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="L67" s="44" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="N67" s="42" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="O67" s="43" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="P67" s="44" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="R67" s="42"/>
       <c r="S67" s="43"/>
@@ -5166,43 +5166,43 @@
     </row>
     <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="B68" s="42" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="C68" s="43" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="D68" s="44" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="F68" s="42" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="G68" s="43" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="H68" s="44" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="J68" s="42" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="K68" s="43" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="L68" s="44" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="N68" s="42" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="O68" s="43" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="P68" s="44" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="R68" s="42"/>
       <c r="S68" s="43"/>
@@ -5219,7 +5219,7 @@
     </row>
     <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="B69" s="42" t="s">
         <v>110</v>
@@ -5272,7 +5272,7 @@
     </row>
     <row r="70" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="B70" s="42" t="s">
         <v>110</v>
@@ -5325,7 +5325,7 @@
     </row>
     <row r="71" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B71" s="42" t="s">
         <v>110</v>
@@ -5378,7 +5378,7 @@
     </row>
     <row r="72" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="B72" s="45" t="s">
         <v>110</v>
@@ -5514,43 +5514,43 @@
     </row>
     <row r="76" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B76" s="42" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C76" s="43" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="D76" s="44" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="F76" s="42" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="G76" s="43" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="H76" s="44" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="J76" s="42" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="K76" s="43" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="L76" s="44" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="N76" s="42" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="O76" s="43" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="P76" s="44" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="R76" s="42"/>
       <c r="S76" s="43"/>
@@ -5567,43 +5567,43 @@
     </row>
     <row r="77" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="B77" s="42" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="C77" s="43" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="D77" s="44" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="F77" s="42" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="G77" s="43" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="H77" s="44" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="J77" s="42" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="K77" s="43" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="L77" s="44" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="N77" s="42" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="O77" s="43" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="P77" s="44" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="R77" s="42"/>
       <c r="S77" s="43"/>
@@ -5620,43 +5620,43 @@
     </row>
     <row r="78" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="B78" s="45" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="C78" s="46" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="D78" s="47" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="F78" s="45" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="G78" s="46" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="H78" s="47" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="J78" s="45" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="K78" s="46" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="L78" s="47" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="N78" s="45" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="O78" s="46" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="P78" s="47" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="R78" s="45"/>
       <c r="S78" s="46"/>
@@ -5756,43 +5756,43 @@
     </row>
     <row r="82" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="B82" s="42" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="C82" s="43" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="D82" s="44" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="F82" s="42" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="G82" s="43" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="H82" s="44" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="J82" s="42" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="K82" s="43" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="L82" s="44" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="N82" s="42" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="O82" s="43" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="P82" s="44" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="R82" s="42"/>
       <c r="S82" s="43"/>
@@ -5809,43 +5809,43 @@
     </row>
     <row r="83" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="B83" s="42" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C83" s="43" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="D83" s="44" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="F83" s="42" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="G83" s="43" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="H83" s="44" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="J83" s="42" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="K83" s="43" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="L83" s="44" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="N83" s="42" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="O83" s="43" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="P83" s="44" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="R83" s="42"/>
       <c r="S83" s="43"/>
@@ -5862,43 +5862,43 @@
     </row>
     <row r="84" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="B84" s="42" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C84" s="43" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="D84" s="44" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="F84" s="42" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="G84" s="43" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="H84" s="44" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="J84" s="42" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="K84" s="43" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="L84" s="44" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="N84" s="42" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="O84" s="43" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="P84" s="44" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="R84" s="42"/>
       <c r="S84" s="43"/>
@@ -5915,43 +5915,43 @@
     </row>
     <row r="85" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="B85" s="42" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="C85" s="43" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="D85" s="44" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="F85" s="42" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="G85" s="43" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="H85" s="44" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="J85" s="42" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="K85" s="43" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="L85" s="44" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="N85" s="42" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="O85" s="43" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="P85" s="44" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="R85" s="42"/>
       <c r="S85" s="43"/>
@@ -5968,43 +5968,43 @@
     </row>
     <row r="86" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="B86" s="45" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="C86" s="46" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="D86" s="47" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="F86" s="45" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="G86" s="46" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="H86" s="47" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="J86" s="45" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="K86" s="46" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="L86" s="47" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="N86" s="45" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="O86" s="46" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="P86" s="47" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="R86" s="45"/>
       <c r="S86" s="46"/>
@@ -6047,7 +6047,7 @@
     </row>
     <row r="88" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="43"/>
@@ -6076,43 +6076,43 @@
     </row>
     <row r="89" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B89" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="C89" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="D89" s="44" t="s">
+        <v>260</v>
+      </c>
+      <c r="F89" s="42" t="s">
+        <v>261</v>
+      </c>
+      <c r="G89" s="43" t="s">
+        <v>262</v>
+      </c>
+      <c r="H89" s="44" t="s">
+        <v>263</v>
+      </c>
+      <c r="J89" s="42" t="s">
+        <v>264</v>
+      </c>
+      <c r="K89" s="43" t="s">
+        <v>265</v>
+      </c>
+      <c r="L89" s="44" t="s">
+        <v>266</v>
+      </c>
+      <c r="N89" s="42" t="s">
+        <v>267</v>
+      </c>
+      <c r="O89" s="43" t="s">
         <v>268</v>
       </c>
-      <c r="B89" s="42" t="s">
+      <c r="P89" s="44" t="s">
         <v>269</v>
-      </c>
-      <c r="C89" s="43" t="s">
-        <v>270</v>
-      </c>
-      <c r="D89" s="44" t="s">
-        <v>271</v>
-      </c>
-      <c r="F89" s="42" t="s">
-        <v>272</v>
-      </c>
-      <c r="G89" s="43" t="s">
-        <v>273</v>
-      </c>
-      <c r="H89" s="44" t="s">
-        <v>274</v>
-      </c>
-      <c r="J89" s="42" t="s">
-        <v>275</v>
-      </c>
-      <c r="K89" s="43" t="s">
-        <v>276</v>
-      </c>
-      <c r="L89" s="44" t="s">
-        <v>277</v>
-      </c>
-      <c r="N89" s="42" t="s">
-        <v>278</v>
-      </c>
-      <c r="O89" s="43" t="s">
-        <v>279</v>
-      </c>
-      <c r="P89" s="44" t="s">
-        <v>280</v>
       </c>
       <c r="R89" s="42"/>
       <c r="S89" s="43"/>
@@ -6129,43 +6129,43 @@
     </row>
     <row r="90" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="B90" s="42" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="C90" s="43" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="D90" s="44" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="F90" s="42" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="G90" s="43" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="H90" s="44" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="J90" s="42" t="s">
+        <v>264</v>
+      </c>
+      <c r="K90" s="43" t="s">
         <v>275</v>
       </c>
-      <c r="K90" s="43" t="s">
-        <v>286</v>
-      </c>
       <c r="L90" s="44" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="N90" s="42" t="s">
+        <v>267</v>
+      </c>
+      <c r="O90" s="43" t="s">
+        <v>277</v>
+      </c>
+      <c r="P90" s="44" t="s">
         <v>278</v>
-      </c>
-      <c r="O90" s="43" t="s">
-        <v>288</v>
-      </c>
-      <c r="P90" s="44" t="s">
-        <v>289</v>
       </c>
       <c r="R90" s="42"/>
       <c r="S90" s="43"/>
@@ -6182,43 +6182,43 @@
     </row>
     <row r="91" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B91" s="42" t="s">
+        <v>280</v>
+      </c>
+      <c r="C91" s="43" t="s">
+        <v>281</v>
+      </c>
+      <c r="D91" s="44" t="s">
+        <v>282</v>
+      </c>
+      <c r="F91" s="42" t="s">
+        <v>283</v>
+      </c>
+      <c r="G91" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="H91" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="J91" s="42" t="s">
+        <v>286</v>
+      </c>
+      <c r="K91" s="43" t="s">
+        <v>287</v>
+      </c>
+      <c r="L91" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="N91" s="42" t="s">
+        <v>289</v>
+      </c>
+      <c r="O91" s="43" t="s">
         <v>290</v>
       </c>
-      <c r="B91" s="42" t="s">
+      <c r="P91" s="44" t="s">
         <v>291</v>
-      </c>
-      <c r="C91" s="43" t="s">
-        <v>292</v>
-      </c>
-      <c r="D91" s="44" t="s">
-        <v>293</v>
-      </c>
-      <c r="F91" s="42" t="s">
-        <v>294</v>
-      </c>
-      <c r="G91" s="43" t="s">
-        <v>295</v>
-      </c>
-      <c r="H91" s="44" t="s">
-        <v>296</v>
-      </c>
-      <c r="J91" s="42" t="s">
-        <v>297</v>
-      </c>
-      <c r="K91" s="43" t="s">
-        <v>298</v>
-      </c>
-      <c r="L91" s="44" t="s">
-        <v>299</v>
-      </c>
-      <c r="N91" s="42" t="s">
-        <v>300</v>
-      </c>
-      <c r="O91" s="43" t="s">
-        <v>301</v>
-      </c>
-      <c r="P91" s="44" t="s">
-        <v>302</v>
       </c>
       <c r="R91" s="42"/>
       <c r="S91" s="43"/>
@@ -6235,7 +6235,7 @@
     </row>
     <row r="92" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="B92" s="42" t="s">
         <v>109</v>
@@ -6288,43 +6288,43 @@
     </row>
     <row r="93" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="B93" s="45" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="C93" s="46" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D93" s="47" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="F93" s="45" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="G93" s="46" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H93" s="47" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="J93" s="45" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="K93" s="46" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="L93" s="47" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="N93" s="45" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="O93" s="46" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="P93" s="47" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="R93" s="45"/>
       <c r="S93" s="46"/>

</xml_diff>